<commit_message>
Updated Data for 2023 and Ran Scripts
</commit_message>
<xml_diff>
--- a/outputs/Combined_TIF_Abatement_Taxes.xlsx
+++ b/outputs/Combined_TIF_Abatement_Taxes.xlsx
@@ -1657,13 +1657,13 @@
         <v>7</v>
       </c>
       <c r="D64" t="n">
-        <v>17388.230393838</v>
+        <v>21683.9361904972</v>
       </c>
       <c r="E64" t="n">
         <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>17388.230393838</v>
+        <v>21683.9361904972</v>
       </c>
     </row>
     <row r="65">
@@ -1677,13 +1677,13 @@
         <v>8</v>
       </c>
       <c r="D65" t="n">
-        <v>100696.059606162</v>
+        <v>125572.693809503</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>100696.059606162</v>
+        <v>125572.693809503</v>
       </c>
     </row>
     <row r="66">
@@ -1697,13 +1697,13 @@
         <v>7</v>
       </c>
       <c r="D66" t="n">
-        <v>9041.8345725848</v>
+        <v>19068.7296387063</v>
       </c>
       <c r="E66" t="n">
-        <v>8580.84748720301</v>
+        <v>13590.8188469453</v>
       </c>
       <c r="F66" t="n">
-        <v>17622.6820597878</v>
+        <v>32659.5484856516</v>
       </c>
     </row>
     <row r="67">
@@ -1717,13 +1717,13 @@
         <v>8</v>
       </c>
       <c r="D67" t="n">
-        <v>37816.7754274152</v>
+        <v>79753.4903612937</v>
       </c>
       <c r="E67" t="n">
-        <v>35888.732512797</v>
+        <v>56842.5511530548</v>
       </c>
       <c r="F67" t="n">
-        <v>73705.5079402122</v>
+        <v>136596.041514349</v>
       </c>
     </row>
     <row r="68">
@@ -1737,13 +1737,13 @@
         <v>7</v>
       </c>
       <c r="D68" t="n">
-        <v>86032.3116580934</v>
+        <v>105386.910561649</v>
       </c>
       <c r="E68" t="n">
-        <v>270.250709221331</v>
+        <v>402.716224242701</v>
       </c>
       <c r="F68" t="n">
-        <v>86302.5623673147</v>
+        <v>105789.626785892</v>
       </c>
     </row>
     <row r="69">
@@ -1757,13 +1757,13 @@
         <v>8</v>
       </c>
       <c r="D69" t="n">
-        <v>604680.598843232</v>
+        <v>747650.279629641</v>
       </c>
       <c r="E69" t="n">
-        <v>1831.09043659686</v>
+        <v>2728.61384526203</v>
       </c>
       <c r="F69" t="n">
-        <v>606511.689279829</v>
+        <v>750378.893474903</v>
       </c>
     </row>
     <row r="70">
@@ -1777,13 +1777,13 @@
         <v>11</v>
       </c>
       <c r="D70" t="n">
-        <v>160288.519498674</v>
+        <v>196577.75980871</v>
       </c>
       <c r="E70" t="n">
-        <v>501.24885418181</v>
+        <v>746.939930495271</v>
       </c>
       <c r="F70" t="n">
-        <v>160789.768352856</v>
+        <v>197324.699739205</v>
       </c>
     </row>
     <row r="71">
@@ -1797,13 +1797,13 @@
         <v>7</v>
       </c>
       <c r="D71" t="n">
-        <v>9440.20490291833</v>
+        <v>13227.6073808706</v>
       </c>
       <c r="E71" t="n">
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>9440.20490291833</v>
+        <v>13227.6073808706</v>
       </c>
     </row>
     <row r="72">
@@ -1817,13 +1817,13 @@
         <v>8</v>
       </c>
       <c r="D72" t="n">
-        <v>90723.1350970817</v>
+        <v>127121.182619129</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>90723.1350970817</v>
+        <v>127121.182619129</v>
       </c>
     </row>
     <row r="73">
@@ -2591,13 +2591,13 @@
         <v>7</v>
       </c>
       <c r="D20" t="n">
-        <v>17388.230393838</v>
+        <v>21683.9361904972</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>17388.230393838</v>
+        <v>21683.9361904972</v>
       </c>
     </row>
     <row r="21">
@@ -2611,13 +2611,13 @@
         <v>8</v>
       </c>
       <c r="D21" t="n">
-        <v>100696.059606162</v>
+        <v>125572.693809503</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>100696.059606162</v>
+        <v>125572.693809503</v>
       </c>
     </row>
     <row r="22">
@@ -3065,13 +3065,13 @@
         <v>7</v>
       </c>
       <c r="D20" t="n">
-        <v>9041.8345725848</v>
+        <v>19068.7296387063</v>
       </c>
       <c r="E20" t="n">
-        <v>8580.84748720301</v>
+        <v>13590.8188469453</v>
       </c>
       <c r="F20" t="n">
-        <v>17622.6820597878</v>
+        <v>32659.5484856516</v>
       </c>
     </row>
     <row r="21">
@@ -3085,13 +3085,13 @@
         <v>8</v>
       </c>
       <c r="D21" t="n">
-        <v>37816.7754274152</v>
+        <v>79753.4903612937</v>
       </c>
       <c r="E21" t="n">
-        <v>35888.732512797</v>
+        <v>56842.5511530548</v>
       </c>
       <c r="F21" t="n">
-        <v>73705.5079402122</v>
+        <v>136596.041514349</v>
       </c>
     </row>
     <row r="22">
@@ -3539,13 +3539,13 @@
         <v>7</v>
       </c>
       <c r="D20" t="n">
-        <v>86032.3116580934</v>
+        <v>105386.910561649</v>
       </c>
       <c r="E20" t="n">
-        <v>270.250709221331</v>
+        <v>402.716224242701</v>
       </c>
       <c r="F20" t="n">
-        <v>86302.5623673147</v>
+        <v>105789.626785892</v>
       </c>
     </row>
     <row r="21">
@@ -3559,13 +3559,13 @@
         <v>8</v>
       </c>
       <c r="D21" t="n">
-        <v>604680.598843232</v>
+        <v>747650.279629641</v>
       </c>
       <c r="E21" t="n">
-        <v>1831.09043659686</v>
+        <v>2728.61384526203</v>
       </c>
       <c r="F21" t="n">
-        <v>606511.689279829</v>
+        <v>750378.893474903</v>
       </c>
     </row>
     <row r="22">
@@ -3579,13 +3579,13 @@
         <v>11</v>
       </c>
       <c r="D22" t="n">
-        <v>160288.519498674</v>
+        <v>196577.75980871</v>
       </c>
       <c r="E22" t="n">
-        <v>501.24885418181</v>
+        <v>746.939930495271</v>
       </c>
       <c r="F22" t="n">
-        <v>160789.768352856</v>
+        <v>197324.699739205</v>
       </c>
     </row>
     <row r="23">
@@ -4033,13 +4033,13 @@
         <v>7</v>
       </c>
       <c r="D10" t="n">
-        <v>9440.20490291833</v>
+        <v>13227.6073808706</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>9440.20490291833</v>
+        <v>13227.6073808706</v>
       </c>
     </row>
     <row r="11">
@@ -4053,13 +4053,13 @@
         <v>8</v>
       </c>
       <c r="D11" t="n">
-        <v>90723.1350970817</v>
+        <v>127121.182619129</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>90723.1350970817</v>
+        <v>127121.182619129</v>
       </c>
     </row>
     <row r="12">

</xml_diff>